<commit_message>
adiciona ultimos experimentos do powell no fim
</commit_message>
<xml_diff>
--- a/experimentação/rosenbrock/Testes_max_fun_calls/experimento_rosen_100_dimensoes_cdeepso.xlsx
+++ b/experimentação/rosenbrock/Testes_max_fun_calls/experimento_rosen_100_dimensoes_cdeepso.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a10f9ab6fab0dff6/Documentos/UFRJ/TCC/powell-cdeepso/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a10f9ab6fab0dff6/Documentos/UFRJ/TCC/powell-cdeepso/experimentação/rosenbrock/Testes_max_fun_calls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_4BA68BC46B741ED3B1C862373E358AD3F29CD82F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83DCAF0E-3419-4DCA-B22A-69A692430BFC}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_4BA68BC46B741ED3B1C862373E358AD3F29CD82F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25D65065-9655-4C82-9709-DFA602F5B382}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -505,7 +505,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>